<commit_message>
modifications and adding test runner
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,66 +19,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
-  <si>
-    <t>johndoe@example.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>secret123</t>
   </si>
   <si>
-    <t>janesmith@example.com</t>
-  </si>
-  <si>
     <t>mypassword123</t>
   </si>
   <si>
     <t>johndoe1@example.com</t>
   </si>
   <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Ebrahim</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
     <t>janesmith1@example.com</t>
   </si>
   <si>
-    <t>TestNG1234</t>
-  </si>
-  <si>
-    <t>TestNG@Framework.com</t>
-  </si>
-  <si>
-    <t>Joe@Doe.com</t>
-  </si>
-  <si>
-    <t>DoeDoe34</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>Mohamed</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Ebrahim</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>LastName</t>
+    <t>johndoe12@example.com</t>
   </si>
 </sst>
 </file>
@@ -123,11 +102,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -410,130 +386,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>